<commit_message>
reading data from excell
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joebr\IdeaProjects\shop-expense-tracker\src\main\java\com\example\shopexpensetracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joebr\IdeaProjects\shop-expense-tracker\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="product-sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -383,7 +383,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
product list and add product section done
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Product ID</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>PD Name 9</t>
+  </si>
+  <si>
+    <t>PD Product 10</t>
+  </si>
+  <si>
+    <t>PD Name 11</t>
+  </si>
+  <si>
+    <t>asdf</t>
   </si>
 </sst>
 </file>
@@ -380,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,6 +540,48 @@
         <v>19</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1212</v>
+      </c>
+      <c r="D12">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>123</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
admin buy product added
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joebr\IdeaProjects\shop-expense-tracker\src\main\resources\data\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,56 +38,55 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>PD Name 1</t>
-  </si>
-  <si>
-    <t>PD Name 2</t>
-  </si>
-  <si>
-    <t>PD Name 3</t>
-  </si>
-  <si>
-    <t>PD Name 4</t>
-  </si>
-  <si>
-    <t>PD Name 5</t>
-  </si>
-  <si>
-    <t>PD Name 6</t>
-  </si>
-  <si>
-    <t>PD Name 7</t>
-  </si>
-  <si>
-    <t>PD Name 8</t>
-  </si>
-  <si>
-    <t>PD Name 9</t>
-  </si>
-  <si>
-    <t>PD Product 10</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>priduct test</t>
-  </si>
-  <si>
-    <t>product test</t>
-  </si>
-  <si>
-    <t>Product test</t>
-  </si>
-  <si>
-    <t>product test test</t>
+    <t>Shop Pd - 1</t>
+  </si>
+  <si>
+    <t>Shop Pd - 2</t>
+  </si>
+  <si>
+    <t>Shop Pd - 3</t>
+  </si>
+  <si>
+    <t>Shop Pd - 4</t>
+  </si>
+  <si>
+    <t>Shop Pd - 5</t>
+  </si>
+  <si>
+    <t>Shop Pd - 6</t>
+  </si>
+  <si>
+    <t>Shop Pd - 7</t>
+  </si>
+  <si>
+    <t>Shop Pd - 8</t>
+  </si>
+  <si>
+    <t>Shop Pd - 9</t>
+  </si>
+  <si>
+    <t>Shop Pd - 10</t>
+  </si>
+  <si>
+    <t>Shop Pd - 11</t>
+  </si>
+  <si>
+    <t>Shop Pd - 12</t>
+  </si>
+  <si>
+    <t>Shop Pd - 13</t>
+  </si>
+  <si>
+    <t>Shop Pd - 14</t>
+  </si>
+  <si>
+    <t>Shop Pd - 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,237 +400,237 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.33203125"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0">
+      <c r="C2">
         <v>12</v>
       </c>
-      <c r="D2" s="0">
+      <c r="D2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0">
+      <c r="C3">
         <v>13</v>
       </c>
-      <c r="D3" s="0">
+      <c r="D3">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>14</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>15</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>16</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>17</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <v>18</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9">
         <v>19</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10">
         <v>20</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11">
         <v>56</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="0">
+      <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="0">
+      <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" s="0">
+      <c r="D12">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="0">
+      <c r="A13">
         <v>14</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="0">
+      <c r="C13">
         <v>2323</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D13">
         <v>232323</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n" s="0">
-        <v>15.0</v>
-      </c>
-      <c r="B14" t="s" s="0">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="n" s="0">
-        <v>121.0</v>
-      </c>
-      <c r="D14" t="n" s="0">
-        <v>121212.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n" s="0">
-        <v>16.0</v>
-      </c>
-      <c r="B15" t="s" s="0">
+      <c r="C14">
+        <v>121</v>
+      </c>
+      <c r="D14">
+        <v>121212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="n" s="0">
-        <v>1212.0</v>
-      </c>
-      <c r="D15" t="n" s="0">
-        <v>1.2121212E7</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n" s="0">
-        <v>17.0</v>
-      </c>
-      <c r="B16" t="s" s="0">
+      <c r="C15">
+        <v>1212</v>
+      </c>
+      <c r="D15">
+        <v>12121212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="n" s="0">
-        <v>2323.0</v>
-      </c>
-      <c r="D16" t="n" s="0">
-        <v>2323.0</v>
+      <c r="C16">
+        <v>2323</v>
+      </c>
+      <c r="D16">
+        <v>2323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function modified for repaing product add
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joebr\IdeaProjects\shop-expense-tracker\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5424"/>
   </bookViews>
   <sheets>
     <sheet name="product-sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Product ID</t>
   </si>
@@ -38,55 +38,44 @@
     <t>Stock</t>
   </si>
   <si>
-    <t>Shop Pd - 1</t>
-  </si>
-  <si>
-    <t>Shop Pd - 2</t>
-  </si>
-  <si>
-    <t>Shop Pd - 3</t>
-  </si>
-  <si>
-    <t>Shop Pd - 4</t>
-  </si>
-  <si>
-    <t>Shop Pd - 5</t>
-  </si>
-  <si>
-    <t>Shop Pd - 6</t>
-  </si>
-  <si>
-    <t>Shop Pd - 7</t>
-  </si>
-  <si>
-    <t>Shop Pd - 8</t>
-  </si>
-  <si>
-    <t>Shop Pd - 9</t>
-  </si>
-  <si>
-    <t>Shop Pd - 10</t>
-  </si>
-  <si>
-    <t>Shop Pd - 11</t>
-  </si>
-  <si>
-    <t>Shop Pd - 12</t>
-  </si>
-  <si>
-    <t>Shop Pd - 13</t>
-  </si>
-  <si>
-    <t>Shop Pd - 14</t>
-  </si>
-  <si>
-    <t>Shop Pd - 15</t>
+    <t>PD Name 1</t>
+  </si>
+  <si>
+    <t>PD Name 2</t>
+  </si>
+  <si>
+    <t>PD Name 3</t>
+  </si>
+  <si>
+    <t>PD Name 4</t>
+  </si>
+  <si>
+    <t>PD Name 5</t>
+  </si>
+  <si>
+    <t>PD Name 6</t>
+  </si>
+  <si>
+    <t>PD Name 7</t>
+  </si>
+  <si>
+    <t>PD Name 8</t>
+  </si>
+  <si>
+    <t>PD Name 9</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD Name 1 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,8 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,242 +390,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" style="2" width="8.88671875"/>
+    <col min="2" max="2" customWidth="true" width="17.33203125"/>
+    <col min="3" max="3" style="1" width="8.88671875"/>
+    <col min="4" max="4" style="2" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>12</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3" t="n">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
         <v>13</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="2">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>56</v>
-      </c>
-      <c r="D11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>2323</v>
-      </c>
-      <c r="D13">
-        <v>232323</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>121</v>
-      </c>
-      <c r="D14">
-        <v>121212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>1212</v>
-      </c>
-      <c r="D15">
-        <v>12121212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>2323</v>
-      </c>
-      <c r="D16">
-        <v>2323</v>
+      <c r="C12" t="n" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="D12" t="n" s="2">
+        <v>12.0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
third party product add successfull
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Product ID</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t xml:space="preserve">PD Name 1 </t>
+  </si>
+  <si>
+    <t>Third Party PD - 1</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>Third Party PD - 5</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
@@ -572,6 +581,48 @@
         <v>12.0</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n" s="2">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C13" t="n" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="D13" t="n" s="2">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C14" t="n" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="D14" t="n" s="2">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C15" t="n" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D15" t="n" s="2">
+        <v>11.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added pay bills section
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Product ID</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>aaa</t>
+  </si>
+  <si>
+    <t>feemicon pill</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -592,10 +595,10 @@
         <v>15</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>57.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -638,6 +641,20 @@
       </c>
       <c r="D16" t="n" s="2">
         <v>1.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C17" t="n" s="1">
+        <v>69.69</v>
+      </c>
+      <c r="D17" t="n" s="2">
+        <v>10000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
decrease product stock when buying or selling
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Product.xlsx
+++ b/src/main/resources/data/Product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Product ID</t>
   </si>
@@ -65,25 +65,19 @@
     <t>PD Name 9</t>
   </si>
   <si>
-    <t>aa</t>
-  </si>
-  <si>
     <t xml:space="preserve">PD Name 1 </t>
   </si>
   <si>
     <t>Third Party PD - 1</t>
   </si>
   <si>
-    <t>as</t>
-  </si>
-  <si>
     <t>Third Party PD - 5</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>feemicon pill</t>
+    <t>Third Party PD - 3</t>
+  </si>
+  <si>
+    <t>Third Party PD - 2</t>
   </si>
 </sst>
 </file>
@@ -123,8 +117,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,17 +410,17 @@
     <col min="1" max="1" style="2" width="8.88671875"/>
     <col min="2" max="2" customWidth="true" width="17.33203125"/>
     <col min="3" max="3" style="1" width="8.88671875"/>
-    <col min="4" max="4" style="2" width="8.88671875"/>
+    <col min="4" max="4" style="3" width="8.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -434,41 +428,41 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>12</v>
       </c>
-      <c r="D2" s="3">
-        <v>54</v>
+      <c r="D2" s="3" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
-        <v>17</v>
+      <c r="D3" s="3" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>14</v>
       </c>
       <c r="D4" s="3">
@@ -476,27 +470,27 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>15</v>
       </c>
-      <c r="D5" s="3">
-        <v>18</v>
+      <c r="D5" s="3" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>16</v>
       </c>
       <c r="D6" s="3">
@@ -504,13 +498,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>17</v>
       </c>
       <c r="D7" s="3">
@@ -518,27 +512,27 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>18</v>
       </c>
-      <c r="D8" s="3">
-        <v>15</v>
+      <c r="D8" s="3" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>19</v>
       </c>
       <c r="D9" s="3">
@@ -546,13 +540,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>20</v>
       </c>
       <c r="D10" s="3">
@@ -560,101 +554,73 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>12</v>
       </c>
       <c r="D11" s="3">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C12" s="1">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>12</v>
+      <c r="C12" s="1" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>110.0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s" s="0">
         <v>15</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>13</v>
+        <v>19.0</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>46.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="2">
+        <v>15.0</v>
       </c>
       <c r="B14" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>13.5</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>14</v>
+      <c r="C14" t="n" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D14" t="n" s="3">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="2">
+        <v>16.0</v>
       </c>
       <c r="B15" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C15" s="1">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n" s="2">
+      <c r="C15" t="n" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="D15" t="n" s="3">
         <v>15.0</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C16" t="n" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="D16" t="n" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n" s="2">
-        <v>16.0</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C17" t="n" s="1">
-        <v>69.69</v>
-      </c>
-      <c r="D17" t="n" s="2">
-        <v>10000.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>